<commit_message>
NEW: Bible api working
</commit_message>
<xml_diff>
--- a/json-project/testdata.xlsx
+++ b/json-project/testdata.xlsx
@@ -27,9 +27,6 @@
     <t>obs</t>
   </si>
   <si>
-    <t>jó</t>
-  </si>
-  <si>
     <t>paciencia</t>
   </si>
   <si>
@@ -39,10 +36,13 @@
     <t>perseverança</t>
   </si>
   <si>
-    <t>abraão</t>
-  </si>
-  <si>
-    <t>teste</t>
+    <t>aliança</t>
+  </si>
+  <si>
+    <t>avraham</t>
+  </si>
+  <si>
+    <t>job</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +408,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -416,10 +416,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -427,10 +427,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>